<commit_message>
Actualiza pasos de git
</commit_message>
<xml_diff>
--- a/Step to Push to GitHub.xlsx
+++ b/Step to Push to GitHub.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnol\Desktop\Proyecto\ProyectoTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C246D55-9350-4984-826B-CE0C3328A041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229D914A-75B8-4C3A-8A3F-6FD8009ECFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>Paso</t>
   </si>
@@ -188,6 +188,60 @@
   </si>
   <si>
     <t>Actualiza el branch master con los cambios del branch nuevo sin crear un nuevo commit</t>
+  </si>
+  <si>
+    <t>git clone https://github.com/YOUR-USERNAME/YOUR-REPOSITORY.git</t>
+  </si>
+  <si>
+    <t>Clona el repositorio remoto en tu PC</t>
+  </si>
+  <si>
+    <t>cd YOUR-REPOSITORY</t>
+  </si>
+  <si>
+    <t>Cambia al directorio del repositorio clonado</t>
+  </si>
+  <si>
+    <t>git status</t>
+  </si>
+  <si>
+    <t>Muestra el estado de los archivos en el repositorio local</t>
+  </si>
+  <si>
+    <t>Agrega todos los archivos modificados al área de preparación</t>
+  </si>
+  <si>
+    <t>git push origin BRANCH-NAME</t>
+  </si>
+  <si>
+    <t>Sube los cambios al repositorio remoto</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>Obtiene la ruta del repositorio original</t>
+  </si>
+  <si>
+    <t>mkdir proyecto-clonado</t>
+  </si>
+  <si>
+    <t>Crea un nuevo directorio llamado proyecto-clonado</t>
+  </si>
+  <si>
+    <t>cd proyecto-clonado</t>
+  </si>
+  <si>
+    <t>Cambia al nuevo directorio</t>
+  </si>
+  <si>
+    <t>git clone /home/user/proyecto-original</t>
+  </si>
+  <si>
+    <t>Clona el repositorio original en el nuevo directorio</t>
+  </si>
+  <si>
+    <t>Clonar un repositorio de GitHub hacia la PC</t>
   </si>
 </sst>
 </file>
@@ -305,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -327,6 +381,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -911,12 +972,174 @@
         <v>32</v>
       </c>
     </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="8"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="5">
+        <v>1</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="5">
+        <v>2</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="5">
+        <v>3</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="5">
+        <v>4</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="5">
+        <v>5</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="5">
+        <v>6</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="11"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="9"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="8"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="5">
+        <v>1</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="5">
+        <v>2</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="5">
+        <v>3</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="5">
+        <v>4</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="5"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A36:B36"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="A1:C6" numberStoredAsText="1"/>
   </ignoredErrors>

</xml_diff>